<commit_message>
Completed missing fields, updated taxonomy
</commit_message>
<xml_diff>
--- a/tabular/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/hepadna-ncbi-refseqs-side-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25540" yWindow="1020" windowWidth="27340" windowHeight="25140" tabRatio="500"/>
+    <workbookView xWindow="8020" yWindow="5280" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="193">
   <si>
     <t>sequence-ID</t>
   </si>
@@ -207,12 +207,6 @@
     <t>Virus</t>
   </si>
   <si>
-    <t>Fish</t>
-  </si>
-  <si>
-    <t>Amphibian</t>
-  </si>
-  <si>
     <t>AY494851</t>
   </si>
   <si>
@@ -261,39 +255,24 @@
     <t>host_common_name</t>
   </si>
   <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t>Nanorana parkeri</t>
   </si>
   <si>
     <t>Tibetan frog</t>
   </si>
   <si>
-    <t>China</t>
-  </si>
-  <si>
     <t>Ardea cinerea</t>
   </si>
   <si>
     <t>Grey heron</t>
   </si>
   <si>
-    <t>Germany</t>
-  </si>
-  <si>
     <t>Psittacula krameri</t>
   </si>
   <si>
     <t>Rose-ringed parakeet</t>
   </si>
   <si>
-    <t>Poland</t>
-  </si>
-  <si>
     <t>Chen rossii</t>
   </si>
   <si>
@@ -312,9 +291,6 @@
     <t>Sheldgoose</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Eudromia elegans </t>
   </si>
   <si>
@@ -363,18 +339,12 @@
     <t>Horseshoe bat</t>
   </si>
   <si>
-    <t>Gabon</t>
-  </si>
-  <si>
     <t>Miniopterus fuliginosus</t>
   </si>
   <si>
     <t>Long-fingered bat</t>
   </si>
   <si>
-    <t>Myanmar</t>
-  </si>
-  <si>
     <t>Hipposideros cf. ruber</t>
   </si>
   <si>
@@ -408,9 +378,6 @@
     <t>Domestic cat</t>
   </si>
   <si>
-    <t>Australia</t>
-  </si>
-  <si>
     <t>U29144</t>
   </si>
   <si>
@@ -426,9 +393,6 @@
     <t>Arctic ground squirrel</t>
   </si>
   <si>
-    <t>Alaska</t>
-  </si>
-  <si>
     <t>SLHBV-1</t>
   </si>
   <si>
@@ -580,6 +544,60 @@
   </si>
   <si>
     <t>Baby whale</t>
+  </si>
+  <si>
+    <t>Unclassified</t>
+  </si>
+  <si>
+    <t>Icefish metahepadnavirus</t>
+  </si>
+  <si>
+    <t>Skink herpetohepadnavirus</t>
+  </si>
+  <si>
+    <t>Astatotilapia nackednavirus</t>
+  </si>
+  <si>
+    <t>Western mosquitofish nackednavirus</t>
+  </si>
+  <si>
+    <t>Spiny lizard herpetohepadnavirus</t>
+  </si>
+  <si>
+    <t>Astatotilapia metahepadnavirus</t>
+  </si>
+  <si>
+    <t>Tetra metahepadnavirus</t>
+  </si>
+  <si>
+    <t>Bluefin killifish nackednavirus</t>
+  </si>
+  <si>
+    <t>Killifish nackednavirus Lp 1</t>
+  </si>
+  <si>
+    <t>Killifish nackednavirus Lp 2</t>
+  </si>
+  <si>
+    <t>European eel nackednavirus</t>
+  </si>
+  <si>
+    <t>Tiger rockfish nackednavirus</t>
+  </si>
+  <si>
+    <t>Baby whale nackednavirus</t>
+  </si>
+  <si>
+    <t>Sockeye salmon nackednavirus</t>
+  </si>
+  <si>
+    <t>Yellow drum nackednavirus</t>
+  </si>
+  <si>
+    <t>Stickleback nackednavirus</t>
+  </si>
+  <si>
+    <t>Coho salmon parahepadnavirus</t>
   </si>
 </sst>
 </file>
@@ -635,7 +653,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -672,6 +690,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -682,7 +724,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="309">
+  <cellStyleXfs count="361">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -992,34 +1034,79 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="309">
+  <cellStyles count="361">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1174,6 +1261,32 @@
     <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1328,6 +1441,32 @@
     <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1657,10 +1796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:A43"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1672,11 +1811,10 @@
     <col min="5" max="5" width="10.83203125" style="2"/>
     <col min="6" max="6" width="28.5" style="2" customWidth="1"/>
     <col min="7" max="7" width="25.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1693,56 +1831,38 @@
         <v>60</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>63</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I2" s="12">
-        <v>40391</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>5</v>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>15</v>
@@ -1750,17 +1870,22 @@
       <c r="E3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>7</v>
+      <c r="F3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>15</v>
@@ -1769,25 +1894,21 @@
         <v>61</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I4" s="13"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>23</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>15</v>
@@ -1796,25 +1917,21 @@
         <v>61</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="I5" s="13"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>16</v>
+        <v>84</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>15</v>
@@ -1823,22 +1940,21 @@
         <v>61</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>20</v>
+        <v>86</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>15</v>
@@ -1847,25 +1963,21 @@
         <v>61</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>19</v>
+        <v>88</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>38</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>15</v>
@@ -1874,851 +1986,814 @@
         <v>61</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G41" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H8" s="2" t="s">
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G9" s="2" t="s">
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I9" s="12">
-        <v>42156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="B43" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I10" s="13"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I11" s="13"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I12" s="13"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I13" s="14">
-        <v>40065</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="D43" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G43" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I14" s="12">
-        <v>41730</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="I15" s="13"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I16" s="13"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I17" s="13"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="I18" s="13">
-        <v>2009</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I19" s="12">
-        <v>39753</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="I20" s="13">
-        <v>2009</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="I21" s="13">
-        <v>2009</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I22" s="13"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="I23" s="13"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="I24" s="14">
-        <v>42464</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="I25" s="13"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>185</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D69">
-    <sortCondition ref="D2:D69"/>
+  <sortState ref="A2:I43">
+    <sortCondition ref="D2:D43"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added the hepadnairusCompound aligner module; added the eSNHBV1 reference for the snakes and aligned the snakes to it
</commit_message>
<xml_diff>
--- a/tabular/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/hepadna-ncbi-refseqs-side-data.xlsx
@@ -1,15 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/DNArt/Hepadnaviridae-GLUE/tabular/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81BF77C-E9D1-0545-A5D0-C1FCF4AE818D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8020" yWindow="5280" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3200" yWindow="1940" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$F$46</definedName>
+  </definedNames>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="195">
   <si>
     <t>sequence-ID</t>
   </si>
@@ -592,12 +601,24 @@
   </si>
   <si>
     <t>Chloephaga poliocephala</t>
+  </si>
+  <si>
+    <t>Colubroidea</t>
+  </si>
+  <si>
+    <t>snakes</t>
+  </si>
+  <si>
+    <t>Endogenous snake hepatitis B virus 1</t>
+  </si>
+  <si>
+    <t>eSNHBV1-con</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1501,6 +1522,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1825,14 +1854,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="A1:F43"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="2" customWidth="1"/>
@@ -1843,7 +1872,7 @@
     <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1863,7 +1892,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>42</v>
       </c>
@@ -1877,7 +1906,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>44</v>
       </c>
@@ -1897,7 +1926,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>50</v>
       </c>
@@ -1917,7 +1946,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>47</v>
       </c>
@@ -1937,7 +1966,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>49</v>
       </c>
@@ -1957,7 +1986,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
@@ -1977,7 +2006,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>59</v>
       </c>
@@ -1997,7 +2026,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>60</v>
       </c>
@@ -2017,7 +2046,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>62</v>
       </c>
@@ -2037,7 +2066,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>66</v>
       </c>
@@ -2057,7 +2086,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>58</v>
       </c>
@@ -2077,7 +2106,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>121</v>
       </c>
@@ -2097,7 +2126,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>125</v>
       </c>
@@ -2117,212 +2146,212 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="16" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B16" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>179</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>129</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>129</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="16" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B19" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>176</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>183</v>
+        <v>145</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>181</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>185</v>
@@ -2337,192 +2366,192 @@
         <v>171</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>188</v>
+        <v>160</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="14" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B31" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C31" s="14" t="s">
         <v>6</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>8</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="F31" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>14</v>
@@ -2531,168 +2560,193 @@
         <v>105</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="E37" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="F37" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>112</v>
+        <v>34</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="F38" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="16" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B40" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C40" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D40" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="16" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B41" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D41" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="14" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B42" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C42" s="14" t="s">
         <v>36</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>32</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>172</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>97</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>172</v>
       </c>
       <c r="E43" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F44" s="6" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:I43">
+  <autoFilter ref="A2:F46" xr:uid="{702386A7-56FA-ED4C-AE43-F9294415061C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F46">
+      <sortCondition ref="D2:D46"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I43">
     <sortCondition ref="D2:D43"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Creating alignment build scripts
</commit_message>
<xml_diff>
--- a/tabular/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/hepadna-ncbi-refseqs-side-data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/DNArt/Hepadnaviridae-GLUE/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81BF77C-E9D1-0545-A5D0-C1FCF4AE818D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3863863-997C-F44C-BC2F-736702D4E89A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="1940" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$F$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$48</definedName>
   </definedNames>
   <calcPr calcId="140000"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="214">
   <si>
     <t>sequence-ID</t>
   </si>
@@ -613,13 +613,70 @@
   </si>
   <si>
     <t>eSNHBV1-con</t>
+  </si>
+  <si>
+    <t>eAVHBV1</t>
+  </si>
+  <si>
+    <t>eAVHBV1-con</t>
+  </si>
+  <si>
+    <t>Endogenous avian hepatitis B virus 1</t>
+  </si>
+  <si>
+    <t>Neognathae</t>
+  </si>
+  <si>
+    <t>birds</t>
+  </si>
+  <si>
+    <t>eCRHBV1</t>
+  </si>
+  <si>
+    <t>eCRHBV2</t>
+  </si>
+  <si>
+    <t>eCRHBV1-con</t>
+  </si>
+  <si>
+    <t>eCRHBV2-con</t>
+  </si>
+  <si>
+    <t>Endogenous crocodile hepatitis B virus 1</t>
+  </si>
+  <si>
+    <t>Endogenous crocodile hepatitis B virus 2</t>
+  </si>
+  <si>
+    <t>Crocodylus</t>
+  </si>
+  <si>
+    <t>crocodiles and gharial</t>
+  </si>
+  <si>
+    <t>eTHBV1</t>
+  </si>
+  <si>
+    <t>eTHBV1-con</t>
+  </si>
+  <si>
+    <t>turtles</t>
+  </si>
+  <si>
+    <t>Endogenous turtle hepatitis B virus 1</t>
+  </si>
+  <si>
+    <t>Chrysemys</t>
+  </si>
+  <si>
+    <t>crocodiles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -648,23 +705,33 @@
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1855,10 +1922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2087,668 +2154,749 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B13" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C13" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>122</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>123</v>
+        <v>76</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>124</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>174</v>
+        <v>121</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>122</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>194</v>
+      <c r="A15" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>125</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>122</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>192</v>
+        <v>126</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>128</v>
+        <v>194</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>129</v>
+        <v>194</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>131</v>
+        <v>191</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>132</v>
+        <v>200</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>132</v>
+        <v>202</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>129</v>
+        <v>204</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>133</v>
+        <v>206</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>134</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>135</v>
+        <v>201</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>135</v>
+        <v>203</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>129</v>
+        <v>205</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>136</v>
+        <v>206</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>137</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>138</v>
+        <v>208</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>70</v>
+        <v>209</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>139</v>
+        <v>212</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>140</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>70</v>
+        <v>178</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>129</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>70</v>
+        <v>179</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>129</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>70</v>
+        <v>173</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>129</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>184</v>
+        <v>141</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>176</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>185</v>
+        <v>144</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>175</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>171</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>185</v>
+        <v>145</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>181</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>186</v>
+        <v>148</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>183</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>187</v>
+        <v>151</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>184</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="F35" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="E38" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="F38" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>111</v>
+        <v>52</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>112</v>
+        <v>27</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D40" s="9" t="s">
+      <c r="A40" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>168</v>
+      <c r="A41" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>169</v>
+        <v>108</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>170</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>92</v>
+        <v>35</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>33</v>
+        <v>112</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>172</v>
+        <v>113</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B48" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C48" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D48" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F44" s="6" t="s">
+      <c r="F48" s="6" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:F46" xr:uid="{702386A7-56FA-ED4C-AE43-F9294415061C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F46">
-      <sortCondition ref="D2:D46"/>
+  <autoFilter ref="A1:F48" xr:uid="{F812D6D6-C044-6B43-8828-F594A1822C8B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F48">
+      <sortCondition ref="D1:D48"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I43">
-    <sortCondition ref="D2:D43"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I44">
+    <sortCondition ref="D2:D44"/>
   </sortState>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Updating/adding reference sequences and alignments
</commit_message>
<xml_diff>
--- a/tabular/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/hepadna-ncbi-refseqs-side-data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/DNArt/Hepadnaviridae-GLUE/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3863863-997C-F44C-BC2F-736702D4E89A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98ACFE6C-BDF8-CC41-9DBC-87AEECC16119}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="660" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$50</definedName>
   </definedNames>
   <calcPr calcId="140000"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="218">
   <si>
     <t>sequence-ID</t>
   </si>
@@ -630,21 +630,12 @@
     <t>birds</t>
   </si>
   <si>
-    <t>eCRHBV1</t>
-  </si>
-  <si>
     <t>eCRHBV2</t>
   </si>
   <si>
-    <t>eCRHBV1-con</t>
-  </si>
-  <si>
     <t>eCRHBV2-con</t>
   </si>
   <si>
-    <t>Endogenous crocodile hepatitis B virus 1</t>
-  </si>
-  <si>
     <t>Endogenous crocodile hepatitis B virus 2</t>
   </si>
   <si>
@@ -654,22 +645,43 @@
     <t>crocodiles and gharial</t>
   </si>
   <si>
-    <t>eTHBV1</t>
-  </si>
-  <si>
-    <t>eTHBV1-con</t>
-  </si>
-  <si>
     <t>turtles</t>
   </si>
   <si>
-    <t>Endogenous turtle hepatitis B virus 1</t>
-  </si>
-  <si>
     <t>Chrysemys</t>
   </si>
   <si>
     <t>crocodiles</t>
+  </si>
+  <si>
+    <t>eCRHBV</t>
+  </si>
+  <si>
+    <t>eCRHBV-con</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endogenous crocodile hepatitis B virus </t>
+  </si>
+  <si>
+    <t>eDRHPV</t>
+  </si>
+  <si>
+    <t>eDRHPV-con</t>
+  </si>
+  <si>
+    <t>Endogenous comodo dragon hepatitis B virus</t>
+  </si>
+  <si>
+    <t>Comodo dragon</t>
+  </si>
+  <si>
+    <t>eTHBV</t>
+  </si>
+  <si>
+    <t>eTHBV-con</t>
+  </si>
+  <si>
+    <t>Endogenous turtle hepatitis B virus</t>
   </si>
 </sst>
 </file>
@@ -1922,10 +1934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:C33"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2255,646 +2267,669 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>122</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>203</v>
-      </c>
       <c r="C18" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>122</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>122</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>128</v>
+        <v>215</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>128</v>
+        <v>216</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>129</v>
+        <v>217</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>130</v>
+        <v>206</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>131</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="10"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>129</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>70</v>
+        <v>132</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>129</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>70</v>
+        <v>173</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>129</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>175</v>
+        <v>138</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E34" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="F37" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="E42" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="F42" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>111</v>
+        <v>46</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E43" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="16" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B46" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C46" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D46" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B47" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D47" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B48" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C48" s="14" t="s">
         <v>36</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>97</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>172</v>
       </c>
       <c r="E48" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="F50" s="6" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F48" xr:uid="{F812D6D6-C044-6B43-8828-F594A1822C8B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F48">
-      <sortCondition ref="D1:D48"/>
+  <autoFilter ref="A1:F50" xr:uid="{F812D6D6-C044-6B43-8828-F594A1822C8B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F50">
+      <sortCondition ref="D1:D50"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I44">
-    <sortCondition ref="D2:D44"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I46">
+    <sortCondition ref="D2:D46"/>
   </sortState>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Further development of build to capture sequence table information for EVEs and EVE genome consensus seqs
</commit_message>
<xml_diff>
--- a/tabular/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/hepadna-ncbi-refseqs-side-data.xlsx
@@ -1,24 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/DNArt/Hepadnaviridae-GLUE/tabular/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB65564-E23E-0C48-A74F-4F57A96CC98E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="660" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21420" yWindow="9960" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$43</definedName>
   </definedNames>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,19 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="222">
-  <si>
-    <t>sequence-ID</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>full_name</t>
-  </si>
-  <si>
-    <t>genus</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="193">
   <si>
     <t>DHBV</t>
   </si>
@@ -603,109 +585,35 @@
     <t>Chloephaga poliocephala</t>
   </si>
   <si>
-    <t>Colubroidea</t>
-  </si>
-  <si>
-    <t>snakes</t>
-  </si>
-  <si>
-    <t>Endogenous snake hepatitis B virus 1</t>
-  </si>
-  <si>
-    <t>eSNHBV1-con</t>
-  </si>
-  <si>
-    <t>eAVHBV1</t>
-  </si>
-  <si>
-    <t>eAVHBV1-con</t>
-  </si>
-  <si>
-    <t>Endogenous avian hepatitis B virus 1</t>
-  </si>
-  <si>
-    <t>Neognathae</t>
-  </si>
-  <si>
-    <t>birds</t>
-  </si>
-  <si>
-    <t>eCRHBV2</t>
-  </si>
-  <si>
-    <t>eCRHBV2-con</t>
-  </si>
-  <si>
-    <t>Endogenous crocodile hepatitis B virus 2</t>
-  </si>
-  <si>
-    <t>Crocodylus</t>
-  </si>
-  <si>
-    <t>crocodiles and gharial</t>
-  </si>
-  <si>
-    <t>turtles</t>
-  </si>
-  <si>
-    <t>Chrysemys</t>
-  </si>
-  <si>
-    <t>crocodiles</t>
-  </si>
-  <si>
-    <t>eCRHBV</t>
-  </si>
-  <si>
-    <t>eCRHBV-con</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endogenous crocodile hepatitis B virus </t>
-  </si>
-  <si>
-    <t>eDRHPV</t>
-  </si>
-  <si>
-    <t>eDRHPV-con</t>
-  </si>
-  <si>
-    <t>Endogenous comodo dragon hepatitis B virus</t>
-  </si>
-  <si>
-    <t>Comodo dragon</t>
-  </si>
-  <si>
-    <t>eTHBV</t>
-  </si>
-  <si>
-    <t>eTHBV-con</t>
-  </si>
-  <si>
-    <t>Endogenous turtle hepatitis B virus</t>
-  </si>
-  <si>
-    <t>SpHBV</t>
-  </si>
-  <si>
-    <t>SphHBV_con</t>
-  </si>
-  <si>
-    <t>Sphenodon hepatitis B virus</t>
-  </si>
-  <si>
-    <t>Sphenodon</t>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>sequenceID</t>
+  </si>
+  <si>
+    <t>virus_name</t>
+  </si>
+  <si>
+    <t>virus_full_name</t>
+  </si>
+  <si>
+    <t>virus_genus</t>
+  </si>
+  <si>
+    <t>clade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -830,8 +738,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="379">
+  <cellStyleXfs count="401">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1230,7 +1160,7 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="379">
+  <cellStyles count="401">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1420,6 +1350,17 @@
     <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1609,6 +1550,17 @@
     <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1945,1013 +1897,924 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A1:XFD1048576"/>
+      <selection activeCell="G1" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="47.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="23.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="25.83203125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="5" width="23.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="8" t="s">
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="8" t="s">
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="G9" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="2" t="s">
+    <row r="11" spans="1:7">
+      <c r="A11" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>198</v>
-      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="10"/>
       <c r="F12" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>37</v>
+        <v>72</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>76</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="E13" s="10"/>
       <c r="F13" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="16" t="s">
         <v>121</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>177</v>
+      <c r="C14" s="16" t="s">
+        <v>170</v>
       </c>
       <c r="D14" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F14" s="2" t="s">
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="16" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>125</v>
-      </c>
       <c r="B15" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="D15" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="16" t="s">
-        <v>194</v>
+        <v>128</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>194</v>
+        <v>128</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="16" t="s">
-        <v>208</v>
+        <v>131</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>209</v>
+        <v>131</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>203</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="11"/>
       <c r="F17" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="16" t="s">
-        <v>200</v>
+        <v>134</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>203</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="12"/>
       <c r="F18" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="16" t="s">
-        <v>211</v>
+        <v>137</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>212</v>
+        <v>137</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="16" t="s">
-        <v>215</v>
+        <v>140</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>216</v>
+        <v>140</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>206</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="12"/>
       <c r="F20" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="16" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>130</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="12"/>
       <c r="F21" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="16" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="D22" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="12"/>
       <c r="F22" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="16" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>136</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="12"/>
       <c r="F23" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="16" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>180</v>
+        <v>150</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>181</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>139</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="E24" s="12"/>
       <c r="F24" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="16" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="12"/>
+      <c r="F25" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="12"/>
+      <c r="F27" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C30" s="16" t="s">
+    <row r="30" spans="1:7">
+      <c r="A30" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="G30" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="G37" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="5"/>
+      <c r="F38" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="9"/>
+      <c r="F39" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C33" s="16" t="s">
+      <c r="D40" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="E40" s="13"/>
+      <c r="F40" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="14" t="s">
+      <c r="E41" s="4"/>
+      <c r="F41" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C42" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>108</v>
-      </c>
+      <c r="D42" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E42" s="4"/>
       <c r="F42" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>14</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E43" s="4"/>
       <c r="F43" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="B46" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
-        <v>218</v>
-      </c>
-      <c r="B47" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="B50" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F50" xr:uid="{1A27AA88-2286-BC47-A07F-AD69D369C957}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F50">
+  <autoFilter ref="A1:G43">
+    <sortState ref="A2:F50">
       <sortCondition ref="D1:D50"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I46">
+  <sortState ref="A2:I46">
     <sortCondition ref="D2:D46"/>
   </sortState>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>

<commit_message>
Fixed incorrect taxonomic labelling in reference data, added new taxa
</commit_message>
<xml_diff>
--- a/tabular/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/hepadna-ncbi-refseqs-side-data.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$45</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="205">
   <si>
     <t>DHBV</t>
   </si>
@@ -528,9 +528,6 @@
     <t>Baby whale</t>
   </si>
   <si>
-    <t>Unclassified</t>
-  </si>
-  <si>
     <t>Icefish metahepadnavirus</t>
   </si>
   <si>
@@ -585,9 +582,6 @@
     <t>Chloephaga poliocephala</t>
   </si>
   <si>
-    <t>Fish</t>
-  </si>
-  <si>
     <t>sequenceID</t>
   </si>
   <si>
@@ -601,6 +595,48 @@
   </si>
   <si>
     <t>clade</t>
+  </si>
+  <si>
+    <t>Eastern sea garfish hepatitis</t>
+  </si>
+  <si>
+    <t>MH716822</t>
+  </si>
+  <si>
+    <t>EsgHBV</t>
+  </si>
+  <si>
+    <t>Eastern sea garfish</t>
+  </si>
+  <si>
+    <t>Hyporhamphus australis</t>
+  </si>
+  <si>
+    <t>RDNV-type</t>
+  </si>
+  <si>
+    <t>SSDNV-type</t>
+  </si>
+  <si>
+    <t>Primate</t>
+  </si>
+  <si>
+    <t>MH484442</t>
+  </si>
+  <si>
+    <t>Shrew hepatitis B virus</t>
+  </si>
+  <si>
+    <t>Crocidura lasiura</t>
+  </si>
+  <si>
+    <t>Ussuri white-toothed shrew</t>
+  </si>
+  <si>
+    <t>ClHBV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lagothrix lagothricha </t>
   </si>
 </sst>
 </file>
@@ -718,13 +754,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -738,8 +774,66 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="413">
+  <cellStyleXfs count="471">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1167,12 +1261,12 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="413">
+  <cellStyles count="471">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1379,6 +1473,35 @@
     <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1585,6 +1708,35 @@
     <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1922,10 +2074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C11" sqref="A11:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1941,19 +2093,19 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>70</v>
@@ -1963,13 +2115,13 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1978,13 +2130,13 @@
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1999,13 +2151,13 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -2020,13 +2172,13 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -2041,13 +2193,13 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -2062,13 +2214,13 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -2076,20 +2228,20 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -2104,13 +2256,13 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -2125,13 +2277,13 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="15" t="s">
         <v>60</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -2146,13 +2298,13 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>64</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -2167,13 +2319,13 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="10" t="s">
@@ -2188,14 +2340,14 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>117</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>118</v>
@@ -2209,14 +2361,14 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>170</v>
+      <c r="C14" s="15" t="s">
+        <v>169</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>118</v>
@@ -2230,612 +2382,688 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C17" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D18" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="C16" s="16" t="s">
+      <c r="E18" s="4"/>
+      <c r="F18" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>171</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="12"/>
+      <c r="E20" s="12" t="s">
+        <v>196</v>
+      </c>
       <c r="F20" s="2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>177</v>
+      <c r="A21" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>171</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="12"/>
+      <c r="E21" s="12" t="s">
+        <v>196</v>
+      </c>
       <c r="F21" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>179</v>
+      <c r="A22" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>170</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="12"/>
+      <c r="E22" s="12" t="s">
+        <v>196</v>
+      </c>
       <c r="F22" s="2" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>180</v>
+      <c r="A23" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>176</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="12"/>
+      <c r="E23" s="12" t="s">
+        <v>196</v>
+      </c>
       <c r="F23" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>181</v>
+      <c r="A24" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>178</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="12"/>
+      <c r="E24" s="12" t="s">
+        <v>196</v>
+      </c>
       <c r="F24" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>181</v>
+      <c r="A25" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>179</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="12"/>
+      <c r="E25" s="12" t="s">
+        <v>196</v>
+      </c>
       <c r="F25" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>182</v>
+      <c r="A26" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="12"/>
+      <c r="E26" s="12" t="s">
+        <v>196</v>
+      </c>
       <c r="F26" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>155</v>
+        <v>69</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>183</v>
+      <c r="A27" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>180</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="12"/>
+      <c r="E27" s="16" t="s">
+        <v>197</v>
+      </c>
       <c r="F27" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>184</v>
+      <c r="A28" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>180</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="12"/>
+      <c r="E28" s="16" t="s">
+        <v>197</v>
+      </c>
       <c r="F28" s="2" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>178</v>
+      <c r="A29" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>181</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="12"/>
+      <c r="E29" s="16" t="s">
+        <v>197</v>
+      </c>
       <c r="F29" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="5"/>
-      <c r="G30" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="14" t="s">
+    <row r="33" spans="1:7">
+      <c r="A33" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B33" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>4</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>20</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="E33" s="5" t="s">
+        <v>198</v>
+      </c>
       <c r="F33" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>22</v>
+      <c r="A34" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="E34" s="5" t="s">
+        <v>198</v>
+      </c>
       <c r="F34" s="2" t="s">
-        <v>101</v>
+        <v>204</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>26</v>
+      <c r="A35" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>2</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E35" s="5"/>
-      <c r="F35" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="G35" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>9</v>
+      <c r="A36" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>31</v>
+      <c r="A37" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E37" s="5"/>
+      <c r="F37" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="G37" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>109</v>
+      <c r="A38" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>22</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="5"/>
+      <c r="F40" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="16" t="s">
+    <row r="42" spans="1:7">
+      <c r="A42" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B43" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C43" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D43" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="9"/>
-      <c r="F39" s="2" t="s">
+      <c r="E43" s="9"/>
+      <c r="F43" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="16" t="s">
+    <row r="44" spans="1:7">
+      <c r="A44" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B44" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D40" s="13" t="s">
+      <c r="C44" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D44" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="2" t="s">
+      <c r="E44" s="11"/>
+      <c r="F44" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="14" t="s">
+    <row r="45" spans="1:7">
+      <c r="A45" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B45" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C45" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="2" t="s">
+      <c r="D45" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E45" s="11"/>
+      <c r="F45" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G45" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:G43">
-    <sortState ref="A2:F50">
-      <sortCondition ref="D1:D50"/>
+  <autoFilter ref="A1:G45">
+    <sortState ref="A2:G45">
+      <sortCondition ref="D2:D45"/>
+      <sortCondition ref="E2:E45"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:I46">

</xml_diff>

<commit_message>
More complete alignment tree rooted in reverse-transcribing elements. Reviewed taxonomy, corrected errors
</commit_message>
<xml_diff>
--- a/tabular/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/hepadna-ncbi-refseqs-side-data.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/Hepadnaviridae-GLUE/tabular/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E662FB-ABDC-004C-B576-095E683D9F96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3200" yWindow="760" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$45</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="206">
   <si>
     <t>DHBV</t>
   </si>
@@ -300,9 +306,6 @@
     <t>White sucker</t>
   </si>
   <si>
-    <t>KX058434</t>
-  </si>
-  <si>
     <t>African cichlid hepadnavirus</t>
   </si>
   <si>
@@ -637,12 +640,18 @@
   </si>
   <si>
     <t>Eastern sea garfish hepatitis B virus</t>
+  </si>
+  <si>
+    <t>virus_family</t>
+  </si>
+  <si>
+    <t>Hepadnaviridae</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2081,48 +2090,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="47.5" style="2" customWidth="1"/>
-    <col min="4" max="5" width="23.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.83203125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="22.5" style="2" customWidth="1"/>
+    <col min="5" max="6" width="23.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="28.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>38</v>
       </c>
@@ -2132,12 +2145,15 @@
       <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>40</v>
       </c>
@@ -2147,18 +2163,21 @@
       <c r="C3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>46</v>
       </c>
@@ -2168,18 +2187,21 @@
       <c r="C4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
@@ -2189,18 +2211,21 @@
       <c r="C5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3"/>
+      <c r="G5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>45</v>
       </c>
@@ -2210,18 +2235,21 @@
       <c r="C6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3"/>
+      <c r="G6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>44</v>
       </c>
@@ -2231,18 +2259,21 @@
       <c r="C7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2" t="s">
-        <v>185</v>
-      </c>
+      <c r="F7" s="3"/>
       <c r="G7" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>55</v>
       </c>
@@ -2252,18 +2283,21 @@
       <c r="C8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3"/>
+      <c r="G8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>56</v>
       </c>
@@ -2273,18 +2307,21 @@
       <c r="C9" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="7"/>
+      <c r="G9" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>58</v>
       </c>
@@ -2294,18 +2331,21 @@
       <c r="C10" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="7"/>
+      <c r="G10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>62</v>
       </c>
@@ -2315,18 +2355,21 @@
       <c r="C11" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="7"/>
+      <c r="G11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>54</v>
       </c>
@@ -2336,60 +2379,69 @@
       <c r="C12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="15" t="s">
+      <c r="H13" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="15" t="s">
+      <c r="F14" s="10"/>
+      <c r="G14" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>53</v>
       </c>
@@ -2399,401 +2451,455 @@
       <c r="C15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="2" t="s">
+      <c r="D15" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>192</v>
-      </c>
       <c r="C16" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="2" t="s">
-        <v>194</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F16" s="4"/>
       <c r="G16" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="F17" s="4"/>
+      <c r="G17" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="F18" s="4"/>
+      <c r="G18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="C20" s="2" t="s">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D23" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D21" s="12" t="s">
+      <c r="F23" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E24" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="D22" s="12" t="s">
+      <c r="F24" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E25" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="15" t="s">
+      <c r="F25" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B25" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>67</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="F26" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="15" t="s">
+      <c r="G27" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="H27" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="H28" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D29" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E29" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D28" s="12" t="s">
+      <c r="F29" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E30" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="D29" s="12" t="s">
+      <c r="F30" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E31" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="D30" s="12" t="s">
+      <c r="F31" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E32" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>41</v>
       </c>
@@ -2803,20 +2909,23 @@
       <c r="C33" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>52</v>
       </c>
@@ -2826,20 +2935,23 @@
       <c r="C34" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>203</v>
+      <c r="F34" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>202</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>39</v>
       </c>
@@ -2849,15 +2961,18 @@
       <c r="C35" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="5"/>
-      <c r="G35" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="F35" s="5"/>
+      <c r="H35" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>49</v>
       </c>
@@ -2867,18 +2982,21 @@
       <c r="C36" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="5"/>
+      <c r="G36" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>47</v>
       </c>
@@ -2888,18 +3006,21 @@
       <c r="C37" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="5"/>
+      <c r="G37" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>48</v>
       </c>
@@ -2909,18 +3030,21 @@
       <c r="C38" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="5"/>
+      <c r="G38" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>50</v>
       </c>
@@ -2930,18 +3054,21 @@
       <c r="C39" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E39" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="2" t="s">
-        <v>101</v>
-      </c>
+      <c r="F39" s="5"/>
       <c r="G39" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>100</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>42</v>
       </c>
@@ -2951,102 +3078,117 @@
       <c r="C40" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="5"/>
+      <c r="G40" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="C41" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="D41" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="H41" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G41" s="2" t="s">
+      <c r="F42" s="5"/>
+      <c r="G42" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="D42" s="5" t="s">
+      <c r="B43" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E43" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="15" t="s">
+      <c r="F43" s="9"/>
+      <c r="G43" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="9"/>
-      <c r="F43" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E44" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="B44" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D44" s="11" t="s">
+      <c r="F44" s="11"/>
+      <c r="G44" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>51</v>
       </c>
@@ -3056,26 +3198,29 @@
       <c r="C45" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D45" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="E45" s="11"/>
-      <c r="F45" s="2" t="s">
+      <c r="D45" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="F45" s="11"/>
+      <c r="G45" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="H45" s="2" t="s">
         <v>91</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G45">
-    <sortState ref="A2:G45">
-      <sortCondition ref="D2:D45"/>
+  <autoFilter ref="A1:H45" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H45">
       <sortCondition ref="E2:E45"/>
+      <sortCondition ref="F2:F45"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:I46">
-    <sortCondition ref="D2:D46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J46">
+    <sortCondition ref="E2:E46"/>
   </sortState>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated Nakednavirus reference to MH158727
</commit_message>
<xml_diff>
--- a/tabular/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/hepadna-ncbi-refseqs-side-data.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="10340" yWindow="0" windowWidth="17340" windowHeight="14460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$45</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="212">
   <si>
     <t>DHBV</t>
   </si>
@@ -300,9 +300,6 @@
     <t>White sucker</t>
   </si>
   <si>
-    <t>KX058434</t>
-  </si>
-  <si>
     <t>African cichlid hepadnavirus</t>
   </si>
   <si>
@@ -652,6 +649,15 @@
   </si>
   <si>
     <t>Pagrus auratus</t>
+  </si>
+  <si>
+    <t>virus_family</t>
+  </si>
+  <si>
+    <t>Hepadnaviridae</t>
+  </si>
+  <si>
+    <t>MH158727</t>
   </si>
 </sst>
 </file>
@@ -789,8 +795,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="505">
+  <cellStyleXfs count="535">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1315,7 +1351,7 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="505">
+  <cellStyles count="535">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1568,6 +1604,21 @@
     <cellStyle name="Followed Hyperlink" xfId="500" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="502" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="504" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="506" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="520" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="522" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="524" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="526" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="528" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="530" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="532" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="534" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1820,6 +1871,21 @@
     <cellStyle name="Hyperlink" xfId="499" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="501" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="503" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="519" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="521" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="523" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="525" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="527" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="529" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="531" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="533" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2157,10 +2223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G43" sqref="A1:G46"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -2168,36 +2234,40 @@
     <col min="1" max="1" width="17.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="47.5" style="2" customWidth="1"/>
-    <col min="4" max="5" width="23.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.83203125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="20.33203125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="23.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="28.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="13" t="s">
         <v>38</v>
       </c>
@@ -2207,12 +2277,15 @@
       <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="13" t="s">
         <v>40</v>
       </c>
@@ -2222,18 +2295,21 @@
       <c r="C3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="13" t="s">
         <v>46</v>
       </c>
@@ -2243,18 +2319,21 @@
       <c r="C4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
@@ -2264,18 +2343,21 @@
       <c r="C5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3"/>
+      <c r="G5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" s="13" t="s">
         <v>45</v>
       </c>
@@ -2285,18 +2367,21 @@
       <c r="C6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3"/>
+      <c r="G6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" s="13" t="s">
         <v>44</v>
       </c>
@@ -2306,18 +2391,21 @@
       <c r="C7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2" t="s">
-        <v>185</v>
-      </c>
+      <c r="F7" s="3"/>
       <c r="G7" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" s="13" t="s">
         <v>55</v>
       </c>
@@ -2327,18 +2415,21 @@
       <c r="C8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3"/>
+      <c r="G8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" s="15" t="s">
         <v>56</v>
       </c>
@@ -2348,18 +2439,21 @@
       <c r="C9" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="7"/>
+      <c r="G9" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" s="15" t="s">
         <v>58</v>
       </c>
@@ -2369,18 +2463,21 @@
       <c r="C10" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="7"/>
+      <c r="G10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="15" t="s">
         <v>62</v>
       </c>
@@ -2390,18 +2487,21 @@
       <c r="C11" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="7"/>
+      <c r="G11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" s="13" t="s">
         <v>54</v>
       </c>
@@ -2411,60 +2511,69 @@
       <c r="C12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="15" t="s">
+      <c r="H13" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="15" t="s">
+      <c r="F14" s="10"/>
+      <c r="G14" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="13" t="s">
         <v>53</v>
       </c>
@@ -2474,401 +2583,455 @@
       <c r="C15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="2" t="s">
+      <c r="D15" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>192</v>
-      </c>
       <c r="C16" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="2" t="s">
-        <v>194</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F16" s="4"/>
       <c r="G16" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="F17" s="4"/>
+      <c r="G17" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="F18" s="4"/>
+      <c r="G18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="C20" s="2" t="s">
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D23" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D21" s="12" t="s">
+      <c r="F23" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E24" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="D22" s="12" t="s">
+      <c r="F24" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E25" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="15" t="s">
+      <c r="F25" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B25" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="15" t="s">
-        <v>92</v>
+        <v>211</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>67</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="F26" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="15" t="s">
+      <c r="G27" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="H27" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="H28" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D29" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E29" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D28" s="12" t="s">
+      <c r="F29" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E30" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="D29" s="12" t="s">
+      <c r="F30" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E31" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="D30" s="12" t="s">
+      <c r="F31" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E32" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="13" t="s">
         <v>41</v>
       </c>
@@ -2878,20 +3041,23 @@
       <c r="C33" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="13" t="s">
         <v>52</v>
       </c>
@@ -2901,20 +3067,23 @@
       <c r="C34" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>203</v>
+      <c r="F34" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>202</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="13" t="s">
         <v>39</v>
       </c>
@@ -2924,15 +3093,18 @@
       <c r="C35" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="5"/>
-      <c r="G35" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="F35" s="5"/>
+      <c r="H35" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="13" t="s">
         <v>49</v>
       </c>
@@ -2942,18 +3114,21 @@
       <c r="C36" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="5"/>
+      <c r="G36" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="13" t="s">
         <v>47</v>
       </c>
@@ -2963,18 +3138,21 @@
       <c r="C37" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="5"/>
+      <c r="G37" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="13" t="s">
         <v>48</v>
       </c>
@@ -2984,18 +3162,21 @@
       <c r="C38" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="5"/>
+      <c r="G38" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="13" t="s">
         <v>50</v>
       </c>
@@ -3005,18 +3186,21 @@
       <c r="C39" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E39" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="2" t="s">
-        <v>101</v>
-      </c>
+      <c r="F39" s="5"/>
       <c r="G39" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>100</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="13" t="s">
         <v>42</v>
       </c>
@@ -3026,102 +3210,117 @@
       <c r="C40" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="5"/>
+      <c r="G40" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="C41" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="D41" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="H41" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G41" s="2" t="s">
+      <c r="F42" s="5"/>
+      <c r="G42" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="15" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="D42" s="5" t="s">
+      <c r="B43" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E43" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="15" t="s">
+      <c r="F43" s="9"/>
+      <c r="G43" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="9"/>
-      <c r="F43" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E44" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="B44" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D44" s="11" t="s">
+      <c r="F44" s="11"/>
+      <c r="G44" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="13" t="s">
         <v>51</v>
       </c>
@@ -3131,47 +3330,53 @@
       <c r="C45" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D45" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="E45" s="11"/>
-      <c r="F45" s="2" t="s">
+      <c r="D45" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="F45" s="11"/>
+      <c r="G45" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="H45" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:8">
       <c r="A46" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="F46" s="11"/>
+      <c r="G46" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="E46" s="11"/>
-      <c r="F46" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>206</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G45">
-    <sortState ref="A2:G45">
-      <sortCondition ref="D2:D45"/>
+  <autoFilter ref="A1:H45">
+    <sortState ref="A2:H45">
       <sortCondition ref="E2:E45"/>
+      <sortCondition ref="F2:F45"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:I46">
-    <sortCondition ref="D2:D46"/>
+  <sortState ref="A2:J46">
+    <sortCondition ref="E2:E46"/>
   </sortState>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>